<commit_message>
Add test 7 into all tests
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test7_Animal/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test7_Animal/ExcelQuery.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="1640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="1641">
   <si>
     <t>Index</t>
   </si>
@@ -3420,9 +3420,6 @@
     <t>stmt s1,s2; assign a; while w; variable v1,v2;</t>
   </si>
   <si>
-    <t>Select &lt;v1,a,v2&gt; such that Parent(w,s1) and Parent(s1,s2) pattern w(v,_) such that Next(s1,s2) and Follows(s2,a) pattern a(v2,_"8"_)</t>
-  </si>
-  <si>
     <t>anaconda 20 antelope,anaconda 24 deer</t>
   </si>
   <si>
@@ -3606,9 +3603,6 @@
     <t>suchthat + suchthat + with + pattern (inverted tuple)</t>
   </si>
   <si>
-    <t>Select &lt;a,s&gt; such that Parent*(a,a) such that Next*(s,a) with a.stmt# = c.value pattern a(_,_"badger"_)</t>
-  </si>
-  <si>
     <t>suchthat + suchthat + with + pattern (inverted suchthat)</t>
   </si>
   <si>
@@ -4945,6 +4939,15 @@
   </si>
   <si>
     <t>12 110 fly anaconda,12 111 jaguar anaconda,12 135 eel anaconda,12 143 earthworm anaconda,12 147 iguana anaconda,12 32 cow anaconda,12 58 deer anaconda,12 99 human anaconda,152 156 flamingo anaconda,152 158 eagle anaconda,152 163 anaconda anaconda,16 110 fly anaconda,16 111 jaguar anaconda,16 135 eel anaconda,16 143 earthworm anaconda,16 147 iguana anaconda,16 32 cow anaconda,16 58 deer anaconda,16 99 human anaconda,164 168 cat anaconda,164 178 cow anaconda,164 181 dog anaconda,173 181 dog anaconda,173 178 cow anaconda</t>
+  </si>
+  <si>
+    <t>Select &lt;a,s&gt; such that Parent*(s,a) such that Next*(a,a) with a.stmt# = c.value pattern a(_,_"badger"_)</t>
+  </si>
+  <si>
+    <t>Select &lt;v1,a,v2&gt; such that Parent(w,s1) and Parent(s1,s2) pattern w(v1,_) such that Next(s1,s2) and Follows(s2,a) pattern a(v2,_"8"_)</t>
+  </si>
+  <si>
+    <t>100 Eleven 14 anaconda 102,100 Eleven 14 anaconda 12,100 Eleven 14 anaconda 139,100 Eleven 14 anaconda 156,100 Eleven 14 anaconda 162,100 Eleven 14 anaconda 20,100 Eleven 14 anaconda 5,100 Eleven 14 anaconda 71,100 Eleven 14 anaconda 84,100 Eleven 14 anaconda 9,100 Eleven 14 anaconda 98,100 Eleven 151 cow 102,100 Eleven 151 cow 12,100 Eleven 151 cow 139,100 Eleven 151 cow 156,100 Eleven 151 cow 162,100 Eleven 151 cow 20,100 Eleven 151 cow 5,100 Eleven 151 cow 71,100 Eleven 151 cow 84,100 Eleven 151 cow 9,100 Eleven 151 cow 98,100 Eleven 154 dog 102,100 Eleven 154 dog 12,100 Eleven 154 dog 139,100 Eleven 154 dog 156,100 Eleven 154 dog 162,100 Eleven 154 dog 20,100 Eleven 154 dog 5,100 Eleven 154 dog 71,100 Eleven 154 dog 84,100 Eleven 154 dog 9,100 Eleven 154 dog 98,100 Eleven 160 earthworm 102,100 Eleven 160 earthworm 12,100 Eleven 160 earthworm 139,100 Eleven 160 earthworm 156,100 Eleven 160 earthworm 162,100 Eleven 160 earthworm 20,100 Eleven 160 earthworm 5,100 Eleven 160 earthworm 71,100 Eleven 160 earthworm 84,100 Eleven 160 earthworm 9,100 Eleven 160 earthworm 98,100 Eleven 171 flamingo 102,100 Eleven 171 flamingo 12,100 Eleven 171 flamingo 139,100 Eleven 171 flamingo 156,100 Eleven 171 flamingo 162,100 Eleven 171 flamingo 20,100 Eleven 171 flamingo 5,100 Eleven 171 flamingo 71,100 Eleven 171 flamingo 84,100 Eleven 171 flamingo 9,100 Eleven 171 flamingo 98,100 Eleven 174 eagle 102,100 Eleven 174 eagle 12,100 Eleven 174 eagle 139,100 Eleven 174 eagle 156,100 Eleven 174 eagle 162,100 Eleven 174 eagle 20,100 Eleven 174 eagle 5,100 Eleven 174 eagle 71,100 Eleven 174 eagle 84,100 Eleven 174 eagle 9,100 Eleven 174 eagle 98,100 Eleven 48 cow 102,100 Eleven 48 cow 12,100 Eleven 48 cow 139,100 Eleven 48 cow 156,100 Eleven 48 cow 162,100 Eleven 48 cow 20,100 Eleven 48 cow 5,100 Eleven 48 cow 71,100 Eleven 48 cow 84,100 Eleven 48 cow 9,100 Eleven 48 cow 98,100 Eleven 54 anaconda 102,100 Eleven 54 anaconda 12,100 Eleven 54 anaconda 139,100 Eleven 54 anaconda 156,100 Eleven 54 anaconda 162,100 Eleven 54 anaconda 20,100 Eleven 54 anaconda 5,100 Eleven 54 anaconda 71,100 Eleven 54 anaconda 84,100 Eleven 54 anaconda 9,100 Eleven 54 anaconda 98,100 Eleven 66 anaconda 102,100 Eleven 66 anaconda 12,100 Eleven 66 anaconda 139,100 Eleven 66 anaconda 156,100 Eleven 66 anaconda 162,100 Eleven 66 anaconda 20,100 Eleven 66 anaconda 5,100 Eleven 66 anaconda 71,100 Eleven 66 anaconda 84,100 Eleven 66 anaconda 9,100 Eleven 66 anaconda 98,100 Eleven 80 cat 102,100 Eleven 80 cat 12,100 Eleven 80 cat 139,100 Eleven 80 cat 156,100 Eleven 80 cat 162,100 Eleven 80 cat 20,100 Eleven 80 cat 5,100 Eleven 80 cat 71,100 Eleven 80 cat 84,100 Eleven 80 cat 9,100 Eleven 80 cat 98,100 Eleven 88 anaconda 102,100 Eleven 88 anaconda 12,100 Eleven 88 anaconda 139,100 Eleven 88 anaconda 156,100 Eleven 88 anaconda 162,100 Eleven 88 anaconda 20,100 Eleven 88 anaconda 5,100 Eleven 88 anaconda 71,100 Eleven 88 anaconda 84,100 Eleven 88 anaconda 9,100 Eleven 88 anaconda 98,100 Eleven 89 cat 102,100 Eleven 89 cat 12,100 Eleven 89 cat 139,100 Eleven 89 cat 156,100 Eleven 89 cat 162,100 Eleven 89 cat 20,100 Eleven 89 cat 5,100 Eleven 89 cat 71,100 Eleven 89 cat 84,100 Eleven 89 cat 9,100 Eleven 89 cat 98,105 Eleven 14 anaconda 102,105 Eleven 14 anaconda 12,105 Eleven 14 anaconda 139,105 Eleven 14 anaconda 156,105 Eleven 14 anaconda 162,105 Eleven 14 anaconda 20,105 Eleven 14 anaconda 5,105 Eleven 14 anaconda 71,105 Eleven 14 anaconda 84,105 Eleven 14 anaconda 9,105 Eleven 14 anaconda 98,105 Eleven 151 cow 102,105 Eleven 151 cow 12,105 Eleven 151 cow 139,105 Eleven 151 cow 156,105 Eleven 151 cow 162,105 Eleven 151 cow 20,105 Eleven 151 cow 5,105 Eleven 151 cow 71,105 Eleven 151 cow 84,105 Eleven 151 cow 9,105 Eleven 151 cow 98,105 Eleven 154 dog 102,105 Eleven 154 dog 12,105 Eleven 154 dog 139,105 Eleven 154 dog 156,105 Eleven 154 dog 162,105 Eleven 154 dog 20,105 Eleven 154 dog 5,105 Eleven 154 dog 71,105 Eleven 154 dog 84,105 Eleven 154 dog 9,105 Eleven 154 dog 98,105 Eleven 160 earthworm 102,105 Eleven 160 earthworm 12,105 Eleven 160 earthworm 139,105 Eleven 160 earthworm 156,105 Eleven 160 earthworm 162,105 Eleven 160 earthworm 20,105 Eleven 160 earthworm 5,105 Eleven 160 earthworm 71,105 Eleven 160 earthworm 84,105 Eleven 160 earthworm 9,105 Eleven 160 earthworm 98,105 Eleven 171 flamingo 102,105 Eleven 171 flamingo 12,105 Eleven 171 flamingo 139,105 Eleven 171 flamingo 156,105 Eleven 171 flamingo 162,105 Eleven 171 flamingo 20,105 Eleven 171 flamingo 5,105 Eleven 171 flamingo 71,105 Eleven 171 flamingo 84,105 Eleven 171 flamingo 9,105 Eleven 171 flamingo 98,105 Eleven 174 eagle 102,105 Eleven 174 eagle 12,105 Eleven 174 eagle 139,105 Eleven 174 eagle 156,105 Eleven 174 eagle 162,105 Eleven 174 eagle 20,105 Eleven 174 eagle 5,105 Eleven 174 eagle 71,105 Eleven 174 eagle 84,105 Eleven 174 eagle 9,105 Eleven 174 eagle 98,105 Eleven 48 cow 102,105 Eleven 48 cow 12,105 Eleven 48 cow 139,105 Eleven 48 cow 156,105 Eleven 48 cow 162,105 Eleven 48 cow 20,105 Eleven 48 cow 5,105 Eleven 48 cow 71,105 Eleven 48 cow 84,105 Eleven 48 cow 9,105 Eleven 48 cow 98,105 Eleven 54 anaconda 102,105 Eleven 54 anaconda 12,105 Eleven 54 anaconda 139,105 Eleven 54 anaconda 156,105 Eleven 54 anaconda 162,105 Eleven 54 anaconda 20,105 Eleven 54 anaconda 5,105 Eleven 54 anaconda 71,105 Eleven 54 anaconda 84,105 Eleven 54 anaconda 9,105 Eleven 54 anaconda 98,105 Eleven 66 anaconda 102,105 Eleven 66 anaconda 12,105 Eleven 66 anaconda 139,105 Eleven 66 anaconda 156,105 Eleven 66 anaconda 162,105 Eleven 66 anaconda 20,105 Eleven 66 anaconda 5,105 Eleven 66 anaconda 71,105 Eleven 66 anaconda 84,105 Eleven 66 anaconda 9,105 Eleven 66 anaconda 98,105 Eleven 80 cat 102,105 Eleven 80 cat 12,105 Eleven 80 cat 139,105 Eleven 80 cat 156,105 Eleven 80 cat 162,105 Eleven 80 cat 20,105 Eleven 80 cat 5,105 Eleven 80 cat 71,105 Eleven 80 cat 84,105 Eleven 80 cat 9,105 Eleven 80 cat 98,105 Eleven 88 anaconda 102,105 Eleven 88 anaconda 12,105 Eleven 88 anaconda 139,105 Eleven 88 anaconda 156,105 Eleven 88 anaconda 162,105 Eleven 88 anaconda 20,105 Eleven 88 anaconda 5,105 Eleven 88 anaconda 71,105 Eleven 88 anaconda 84,105 Eleven 88 anaconda 9,105 Eleven 88 anaconda 98,105 Eleven 89 cat 102,105 Eleven 89 cat 12,105 Eleven 89 cat 139,105 Eleven 89 cat 156,105 Eleven 89 cat 162,105 Eleven 89 cat 20,105 Eleven 89 cat 5,105 Eleven 89 cat 71,105 Eleven 89 cat 84,105 Eleven 89 cat 9,105 Eleven 89 cat 98,11 Eleven 14 anaconda 102,11 Eleven 14 anaconda 12,11 Eleven 14 anaconda 139,11 Eleven 14 anaconda 156,11 Eleven 14 anaconda 162,11 Eleven 14 anaconda 20,11 Eleven 14 anaconda 5,11 Eleven 14 anaconda 71,11 Eleven 14 anaconda 84,11 Eleven 14 anaconda 9,11 Eleven 14 anaconda 98,11 Eleven 151 cow 102,11 Eleven 151 cow 12,11 Eleven 151 cow 139,11 Eleven 151 cow 156,11 Eleven 151 cow 162,11 Eleven 151 cow 20,11 Eleven 151 cow 5,11 Eleven 151 cow 71,11 Eleven 151 cow 84,11 Eleven 151 cow 9,11 Eleven 151 cow 98,11 Eleven 154 dog 102,11 Eleven 154 dog 12,11 Eleven 154 dog 139,11 Eleven 154 dog 156,11 Eleven 154 dog 162,11 Eleven 154 dog 20,11 Eleven 154 dog 5,11 Eleven 154 dog 71,11 Eleven 154 dog 84,11 Eleven 154 dog 9,11 Eleven 154 dog 98,11 Eleven 160 earthworm 102,11 Eleven 160 earthworm 12,11 Eleven 160 earthworm 139,11 Eleven 160 earthworm 156,11 Eleven 160 earthworm 162,11 Eleven 160 earthworm 20,11 Eleven 160 earthworm 5,11 Eleven 160 earthworm 71,11 Eleven 160 earthworm 84,11 Eleven 160 earthworm 9,11 Eleven 160 earthworm 98,11 Eleven 171 flamingo 102,11 Eleven 171 flamingo 12,11 Eleven 171 flamingo 139,11 Eleven 171 flamingo 156,11 Eleven 171 flamingo 162,11 Eleven 171 flamingo 20,11 Eleven 171 flamingo 5,11 Eleven 171 flamingo 71,11 Eleven 171 flamingo 84,11 Eleven 171 flamingo 9,11 Eleven 171 flamingo 98,11 Eleven 174 eagle 102,11 Eleven 174 eagle 12,11 Eleven 174 eagle 139,11 Eleven 174 eagle 156,11 Eleven 174 eagle 162,11 Eleven 174 eagle 20,11 Eleven 174 eagle 5,11 Eleven 174 eagle 71,11 Eleven 174 eagle 84,11 Eleven 174 eagle 9,11 Eleven 174 eagle 98,11 Eleven 48 cow 102,11 Eleven 48 cow 12,11 Eleven 48 cow 139,11 Eleven 48 cow 156,11 Eleven 48 cow 162,11 Eleven 48 cow 20,11 Eleven 48 cow 5,11 Eleven 48 cow 71,11 Eleven 48 cow 84,11 Eleven 48 cow 9,11 Eleven 48 cow 98,11 Eleven 54 anaconda 102,11 Eleven 54 anaconda 12,11 Eleven 54 anaconda 139,11 Eleven 54 anaconda 156,11 Eleven 54 anaconda 162,11 Eleven 54 anaconda 20,11 Eleven 54 anaconda 5,11 Eleven 54 anaconda 71,11 Eleven 54 anaconda 84,11 Eleven 54 anaconda 9,11 Eleven 54 anaconda 98,11 Eleven 66 anaconda 102,11 Eleven 66 anaconda 12,11 Eleven 66 anaconda 139,11 Eleven 66 anaconda 156,11 Eleven 66 anaconda 162,11 Eleven 66 anaconda 20,11 Eleven 66 anaconda 5,11 Eleven 66 anaconda 71,11 Eleven 66 anaconda 84,11 Eleven 66 anaconda 9,11 Eleven 66 anaconda 98,11 Eleven 80 cat 102,11 Eleven 80 cat 12,11 Eleven 80 cat 139,11 Eleven 80 cat 156,11 Eleven 80 cat 162,11 Eleven 80 cat 20,11 Eleven 80 cat 5,11 Eleven 80 cat 71,11 Eleven 80 cat 84,11 Eleven 80 cat 9,11 Eleven 80 cat 98,11 Eleven 88 anaconda 102,11 Eleven 88 anaconda 12,11 Eleven 88 anaconda 139,11 Eleven 88 anaconda 156,11 Eleven 88 anaconda 162,11 Eleven 88 anaconda 20,11 Eleven 88 anaconda 5,11 Eleven 88 anaconda 71,11 Eleven 88 anaconda 84,11 Eleven 88 anaconda 9,11 Eleven 88 anaconda 98,11 Eleven 89 cat 102,11 Eleven 89 cat 12,11 Eleven 89 cat 139,11 Eleven 89 cat 156,11 Eleven 89 cat 162,11 Eleven 89 cat 20,11 Eleven 89 cat 5,11 Eleven 89 cat 71,11 Eleven 89 cat 84,11 Eleven 89 cat 9,11 Eleven 89 cat 98,51 Eleven 14 anaconda 102,51 Eleven 14 anaconda 12,51 Eleven 14 anaconda 139,51 Eleven 14 anaconda 156,51 Eleven 14 anaconda 162,51 Eleven 14 anaconda 20,51 Eleven 14 anaconda 5,51 Eleven 14 anaconda 71,51 Eleven 14 anaconda 84,51 Eleven 14 anaconda 9,51 Eleven 14 anaconda 98,51 Eleven 151 cow 102,51 Eleven 151 cow 12,51 Eleven 151 cow 139,51 Eleven 151 cow 156,51 Eleven 151 cow 162,51 Eleven 151 cow 20,51 Eleven 151 cow 5,51 Eleven 151 cow 71,51 Eleven 151 cow 84,51 Eleven 151 cow 9,51 Eleven 151 cow 98,51 Eleven 154 dog 102,51 Eleven 154 dog 12,51 Eleven 154 dog 139,51 Eleven 154 dog 156,51 Eleven 154 dog 162,51 Eleven 154 dog 20,51 Eleven 154 dog 5,51 Eleven 154 dog 71,51 Eleven 154 dog 84,51 Eleven 154 dog 9,51 Eleven 154 dog 98,51 Eleven 160 earthworm 102,51 Eleven 160 earthworm 12,51 Eleven 160 earthworm 139,51 Eleven 160 earthworm 156,51 Eleven 160 earthworm 162,51 Eleven 160 earthworm 20,51 Eleven 160 earthworm 5,51 Eleven 160 earthworm 71,51 Eleven 160 earthworm 84,51 Eleven 160 earthworm 9,51 Eleven 160 earthworm 98,51 Eleven 171 flamingo 102,51 Eleven 171 flamingo 12,51 Eleven 171 flamingo 139,51 Eleven 171 flamingo 156,51 Eleven 171 flamingo 162,51 Eleven 171 flamingo 20,51 Eleven 171 flamingo 5,51 Eleven 171 flamingo 71,51 Eleven 171 flamingo 84,51 Eleven 171 flamingo 9,51 Eleven 171 flamingo 98,51 Eleven 174 eagle 102,51 Eleven 174 eagle 12,51 Eleven 174 eagle 139,51 Eleven 174 eagle 156,51 Eleven 174 eagle 162,51 Eleven 174 eagle 20,51 Eleven 174 eagle 5,51 Eleven 174 eagle 71,51 Eleven 174 eagle 84,51 Eleven 174 eagle 9,51 Eleven 174 eagle 98,51 Eleven 48 cow 102,51 Eleven 48 cow 12,51 Eleven 48 cow 139,51 Eleven 48 cow 156,51 Eleven 48 cow 162,51 Eleven 48 cow 20,51 Eleven 48 cow 5,51 Eleven 48 cow 71,51 Eleven 48 cow 84,51 Eleven 48 cow 9,51 Eleven 48 cow 98,51 Eleven 54 anaconda 102,51 Eleven 54 anaconda 12,51 Eleven 54 anaconda 139,51 Eleven 54 anaconda 156,51 Eleven 54 anaconda 162,51 Eleven 54 anaconda 20,51 Eleven 54 anaconda 5,51 Eleven 54 anaconda 71,51 Eleven 54 anaconda 84,51 Eleven 54 anaconda 9,51 Eleven 54 anaconda 98,51 Eleven 66 anaconda 102,51 Eleven 66 anaconda 12,51 Eleven 66 anaconda 139,51 Eleven 66 anaconda 156,51 Eleven 66 anaconda 162,51 Eleven 66 anaconda 20,51 Eleven 66 anaconda 5,51 Eleven 66 anaconda 71,51 Eleven 66 anaconda 84,51 Eleven 66 anaconda 9,51 Eleven 66 anaconda 98,51 Eleven 80 cat 102,51 Eleven 80 cat 12,51 Eleven 80 cat 139,51 Eleven 80 cat 156,51 Eleven 80 cat 162,51 Eleven 80 cat 20,51 Eleven 80 cat 5,51 Eleven 80 cat 71,51 Eleven 80 cat 84,51 Eleven 80 cat 9,51 Eleven 80 cat 98,51 Eleven 88 anaconda 102,51 Eleven 88 anaconda 12,51 Eleven 88 anaconda 139,51 Eleven 88 anaconda 156,51 Eleven 88 anaconda 162,51 Eleven 88 anaconda 20,51 Eleven 88 anaconda 5,51 Eleven 88 anaconda 71,51 Eleven 88 anaconda 84,51 Eleven 88 anaconda 9,51 Eleven 88 anaconda 98,51 Eleven 89 cat 102,51 Eleven 89 cat 12,51 Eleven 89 cat 139,51 Eleven 89 cat 156,51 Eleven 89 cat 162,51 Eleven 89 cat 20,51 Eleven 89 cat 5,51 Eleven 89 cat 71,51 Eleven 89 cat 84,51 Eleven 89 cat 9,51 Eleven 89 cat 98</t>
   </si>
 </sst>
 </file>
@@ -5050,7 +5053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5235,6 +5238,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5584,9 +5590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D202" sqref="D202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5736,7 +5742,7 @@
         <v>1117</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>290</v>
+        <v>1640</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>1120</v>
@@ -8072,7 +8078,7 @@
         <v>421</v>
       </c>
       <c r="D64" s="65" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="E64" s="49" t="s">
         <v>422</v>
@@ -8345,7 +8351,7 @@
         <v>445</v>
       </c>
       <c r="D71" s="47" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="E71" s="49" t="s">
         <v>441</v>
@@ -8696,7 +8702,7 @@
         <v>494</v>
       </c>
       <c r="D80" s="65" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="E80" s="49" t="s">
         <v>496</v>
@@ -8729,7 +8735,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="55" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="C81" s="49" t="s">
         <v>500</v>
@@ -8768,7 +8774,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="55" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="C82" s="70" t="s">
         <v>507</v>
@@ -8807,10 +8813,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="55" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C83" s="70" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="D83" s="42" t="s">
         <v>22</v>
@@ -8846,7 +8852,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="55" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="C84" s="49" t="s">
         <v>514</v>
@@ -9515,7 +9521,7 @@
         <v>571</v>
       </c>
       <c r="D101" s="47" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="E101" s="49"/>
       <c r="F101" s="57"/>
@@ -9626,7 +9632,7 @@
         <v>577</v>
       </c>
       <c r="D104" s="47" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="E104" s="49"/>
       <c r="F104" s="57"/>
@@ -9697,7 +9703,7 @@
         <v>580</v>
       </c>
       <c r="C106" s="70" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="D106" s="54" t="s">
         <v>581</v>
@@ -9737,7 +9743,7 @@
         <v>583</v>
       </c>
       <c r="D107" s="68" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="E107" s="49" t="s">
         <v>584</v>
@@ -9776,7 +9782,7 @@
         <v>585</v>
       </c>
       <c r="D108" s="68" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="E108" s="49" t="s">
         <v>586</v>
@@ -9970,7 +9976,7 @@
         <v>49</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="D113" s="41" t="s">
         <v>365</v>
@@ -10369,7 +10375,7 @@
         <v>622</v>
       </c>
       <c r="D123" s="41" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="E123" s="40" t="s">
         <v>623</v>
@@ -10404,13 +10410,13 @@
         <v>123</v>
       </c>
       <c r="B124" s="39" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="C124" s="40" t="s">
         <v>626</v>
       </c>
       <c r="D124" s="41" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="E124" s="40" t="s">
         <v>627</v>
@@ -10771,7 +10777,7 @@
         <v>657</v>
       </c>
       <c r="D133" s="47" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="E133" s="49" t="s">
         <v>658</v>
@@ -10961,7 +10967,7 @@
         <v>27</v>
       </c>
       <c r="C138" s="70" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="D138" s="50" t="s">
         <v>85</v>
@@ -11118,7 +11124,7 @@
         <v>679</v>
       </c>
       <c r="D142" s="47" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="E142" s="49" t="s">
         <v>680</v>
@@ -11194,7 +11200,7 @@
         <v>685</v>
       </c>
       <c r="D144" s="47" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="E144" s="49" t="s">
         <v>686</v>
@@ -11312,7 +11318,7 @@
         <v>692</v>
       </c>
       <c r="D147" s="47" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="E147" s="58" t="s">
         <v>693</v>
@@ -11384,13 +11390,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="55" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="C149" s="49" t="s">
         <v>697</v>
       </c>
       <c r="D149" s="65" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="E149" s="49" t="s">
         <v>696</v>
@@ -11510,7 +11516,7 @@
         <v>704</v>
       </c>
       <c r="C152" s="70" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="D152" s="51" t="s">
         <v>705</v>
@@ -11554,7 +11560,7 @@
         <v>706</v>
       </c>
       <c r="D153" s="68" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="E153" s="49" t="s">
         <v>707</v>
@@ -11882,7 +11888,7 @@
         <v>754</v>
       </c>
       <c r="D161" s="65" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="E161" s="49" t="s">
         <v>715</v>
@@ -11958,13 +11964,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C163" s="70" t="s">
         <v>770</v>
       </c>
       <c r="D163" s="68" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="E163" s="49" t="s">
         <v>712</v>
@@ -12164,7 +12170,7 @@
         <v>804</v>
       </c>
       <c r="D168" s="57" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="E168" s="49" t="s">
         <v>807</v>
@@ -12205,7 +12211,7 @@
         <v>813</v>
       </c>
       <c r="D169" s="42" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="E169" s="49" t="s">
         <v>815</v>
@@ -12328,7 +12334,7 @@
         <v>839</v>
       </c>
       <c r="D172" s="42" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="E172" s="49" t="s">
         <v>832</v>
@@ -12369,7 +12375,7 @@
         <v>845</v>
       </c>
       <c r="D173" s="65" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="E173" s="49" t="s">
         <v>832</v>
@@ -12410,7 +12416,7 @@
         <v>853</v>
       </c>
       <c r="D174" s="47" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="E174" s="49" t="s">
         <v>832</v>
@@ -12448,10 +12454,10 @@
         <v>860</v>
       </c>
       <c r="C175" s="70" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="D175" s="57" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="E175" s="49" t="s">
         <v>863</v>
@@ -12533,7 +12539,7 @@
         <v>874</v>
       </c>
       <c r="D177" s="65" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="E177" s="40" t="s">
         <v>876</v>
@@ -12812,13 +12818,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="55" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="C184" s="49" t="s">
         <v>948</v>
       </c>
       <c r="D184" s="57" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="E184" s="57" t="s">
         <v>950</v>
@@ -12972,7 +12978,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="55" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="C188" s="49" t="s">
         <v>982</v>
@@ -13054,7 +13060,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="55" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="C190" s="49" t="s">
         <v>999</v>
@@ -13182,7 +13188,7 @@
         <v>1026</v>
       </c>
       <c r="D193" s="68" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="E193" s="49" t="s">
         <v>715</v>
@@ -13256,7 +13262,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="55" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="C195" s="49" t="s">
         <v>1041</v>
@@ -13296,13 +13302,13 @@
         <v>195</v>
       </c>
       <c r="B196" s="55" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="C196" s="49" t="s">
         <v>1049</v>
       </c>
       <c r="D196" s="65" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="E196" s="49" t="s">
         <v>1050</v>
@@ -13340,10 +13346,10 @@
         <v>1053</v>
       </c>
       <c r="C197" s="70" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="D197" s="42" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="E197" s="49" t="s">
         <v>1058</v>
@@ -13384,7 +13390,7 @@
         <v>1065</v>
       </c>
       <c r="D198" s="42" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="E198" s="49" t="s">
         <v>1066</v>
@@ -13425,7 +13431,7 @@
         <v>1077</v>
       </c>
       <c r="D199" s="42" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="E199" s="51" t="s">
         <v>1079</v>
@@ -13463,10 +13469,10 @@
         <v>1082</v>
       </c>
       <c r="C200" s="70" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="D200" s="42" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="E200" s="51" t="s">
         <v>1085</v>
@@ -13507,7 +13513,7 @@
         <v>1089</v>
       </c>
       <c r="D201" s="42" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="E201" s="51" t="s">
         <v>1091</v>
@@ -13542,13 +13548,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="55" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="C202" s="49" t="s">
         <v>1096</v>
       </c>
       <c r="D202" s="42" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="E202" s="51" t="s">
         <v>1098</v>
@@ -13589,7 +13595,7 @@
         <v>1102</v>
       </c>
       <c r="D203" s="42" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="E203" s="51" t="s">
         <v>1104</v>
@@ -13630,7 +13636,7 @@
         <v>1110</v>
       </c>
       <c r="D204" s="42" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="E204" s="55" t="s">
         <v>1112</v>
@@ -13749,17 +13755,17 @@
       <c r="B207" s="48" t="s">
         <v>1130</v>
       </c>
-      <c r="C207" s="59" t="s">
+      <c r="C207" s="71" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D207" s="51" t="s">
         <v>1131</v>
       </c>
-      <c r="D207" s="51" t="s">
+      <c r="E207" s="51" t="s">
         <v>1132</v>
       </c>
-      <c r="E207" s="51" t="s">
-        <v>1133</v>
-      </c>
       <c r="F207" s="51" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G207" s="52"/>
       <c r="H207" s="48"/>
@@ -13788,19 +13794,19 @@
         <v>207</v>
       </c>
       <c r="B208" s="48" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C208" s="49" t="s">
         <v>1134</v>
-      </c>
-      <c r="C208" s="49" t="s">
-        <v>1135</v>
       </c>
       <c r="D208" s="51" t="s">
         <v>95</v>
       </c>
       <c r="E208" s="51" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F208" s="51" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G208" s="52"/>
       <c r="H208" s="48"/>
@@ -13829,19 +13835,19 @@
         <v>208</v>
       </c>
       <c r="B209" s="48" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C209" s="49" t="s">
         <v>1137</v>
       </c>
-      <c r="C209" s="49" t="s">
+      <c r="D209" s="51" t="s">
         <v>1138</v>
       </c>
-      <c r="D209" s="51" t="s">
+      <c r="E209" s="51" t="s">
         <v>1139</v>
       </c>
-      <c r="E209" s="51" t="s">
-        <v>1140</v>
-      </c>
       <c r="F209" s="51" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G209" s="52"/>
       <c r="H209" s="48"/>
@@ -13873,16 +13879,16 @@
         <v>1122</v>
       </c>
       <c r="C210" s="49" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D210" s="47" t="s">
         <v>1141</v>
       </c>
-      <c r="D210" s="47" t="s">
+      <c r="E210" s="57" t="s">
         <v>1142</v>
       </c>
-      <c r="E210" s="57" t="s">
-        <v>1143</v>
-      </c>
       <c r="F210" s="57" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G210" s="48"/>
       <c r="H210" s="52"/>
@@ -13911,19 +13917,19 @@
         <v>210</v>
       </c>
       <c r="B211" s="48" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C211" s="49" t="s">
         <v>1144</v>
       </c>
-      <c r="C211" s="49" t="s">
+      <c r="D211" s="54" t="s">
         <v>1145</v>
-      </c>
-      <c r="D211" s="54" t="s">
-        <v>1146</v>
       </c>
       <c r="E211" s="58" t="s">
         <v>715</v>
       </c>
       <c r="F211" s="57" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G211" s="48"/>
       <c r="H211" s="52"/>
@@ -13952,19 +13958,19 @@
         <v>211</v>
       </c>
       <c r="B212" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C212" s="49" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D212" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E212" s="58" t="s">
         <v>1148</v>
       </c>
-      <c r="D212" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E212" s="58" t="s">
+      <c r="F212" s="57" t="s">
         <v>1149</v>
-      </c>
-      <c r="F212" s="57" t="s">
-        <v>1150</v>
       </c>
       <c r="G212" s="48"/>
       <c r="H212" s="52"/>
@@ -13993,19 +13999,19 @@
         <v>212</v>
       </c>
       <c r="B213" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C213" s="49" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D213" s="54" t="s">
         <v>1151</v>
       </c>
-      <c r="D213" s="54" t="s">
+      <c r="E213" s="58" t="s">
         <v>1152</v>
       </c>
-      <c r="E213" s="58" t="s">
-        <v>1153</v>
-      </c>
       <c r="F213" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G213" s="48"/>
       <c r="H213" s="52"/>
@@ -14034,19 +14040,19 @@
         <v>213</v>
       </c>
       <c r="B214" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C214" s="49" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D214" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E214" s="58" t="s">
         <v>1154</v>
       </c>
-      <c r="D214" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E214" s="58" t="s">
-        <v>1155</v>
-      </c>
       <c r="F214" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G214" s="48"/>
       <c r="H214" s="52"/>
@@ -14075,19 +14081,19 @@
         <v>214</v>
       </c>
       <c r="B215" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C215" s="49" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D215" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E215" s="58" t="s">
         <v>1156</v>
       </c>
-      <c r="D215" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E215" s="58" t="s">
-        <v>1157</v>
-      </c>
       <c r="F215" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G215" s="48"/>
       <c r="H215" s="52"/>
@@ -14116,19 +14122,19 @@
         <v>215</v>
       </c>
       <c r="B216" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C216" s="49" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D216" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E216" s="58" t="s">
         <v>1158</v>
       </c>
-      <c r="D216" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E216" s="58" t="s">
-        <v>1159</v>
-      </c>
       <c r="F216" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G216" s="48"/>
       <c r="H216" s="52"/>
@@ -14157,19 +14163,19 @@
         <v>216</v>
       </c>
       <c r="B217" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C217" s="49" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D217" s="54" t="s">
         <v>1160</v>
       </c>
-      <c r="D217" s="54" t="s">
-        <v>1161</v>
-      </c>
       <c r="E217" s="58" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="F217" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G217" s="48"/>
       <c r="H217" s="52"/>
@@ -14198,19 +14204,19 @@
         <v>217</v>
       </c>
       <c r="B218" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C218" s="49" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D218" s="54" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E218" s="58" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="F218" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G218" s="48"/>
       <c r="H218" s="52"/>
@@ -14239,19 +14245,19 @@
         <v>218</v>
       </c>
       <c r="B219" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C219" s="49" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D219" s="54" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E219" s="58" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="F219" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G219" s="48"/>
       <c r="H219" s="52"/>
@@ -14280,19 +14286,19 @@
         <v>219</v>
       </c>
       <c r="B220" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C220" s="49" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D220" s="54" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E220" s="58" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="F220" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G220" s="48"/>
       <c r="H220" s="52"/>
@@ -14321,19 +14327,19 @@
         <v>220</v>
       </c>
       <c r="B221" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C221" s="49" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D221" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E221" s="58" t="s">
         <v>1165</v>
       </c>
-      <c r="D221" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E221" s="58" t="s">
-        <v>1166</v>
-      </c>
       <c r="F221" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G221" s="48"/>
       <c r="H221" s="52"/>
@@ -14362,19 +14368,19 @@
         <v>221</v>
       </c>
       <c r="B222" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C222" s="49" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D222" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E222" s="58" t="s">
         <v>1167</v>
       </c>
-      <c r="D222" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E222" s="58" t="s">
-        <v>1168</v>
-      </c>
       <c r="F222" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G222" s="48"/>
       <c r="H222" s="52"/>
@@ -14403,19 +14409,19 @@
         <v>222</v>
       </c>
       <c r="B223" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C223" s="49" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="D223" s="54" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E223" s="58" t="s">
         <v>712</v>
       </c>
       <c r="F223" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G223" s="48"/>
       <c r="H223" s="52"/>
@@ -14444,19 +14450,19 @@
         <v>223</v>
       </c>
       <c r="B224" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C224" s="49" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D224" s="54" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E224" s="58" t="s">
         <v>741</v>
       </c>
       <c r="F224" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G224" s="48"/>
       <c r="H224" s="52"/>
@@ -14485,19 +14491,19 @@
         <v>224</v>
       </c>
       <c r="B225" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C225" s="49" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D225" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E225" s="58" t="s">
         <v>1171</v>
       </c>
-      <c r="D225" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E225" s="58" t="s">
-        <v>1172</v>
-      </c>
       <c r="F225" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G225" s="48"/>
       <c r="H225" s="52"/>
@@ -14526,19 +14532,19 @@
         <v>225</v>
       </c>
       <c r="B226" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C226" s="49" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D226" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E226" s="58" t="s">
         <v>1173</v>
       </c>
-      <c r="D226" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E226" s="58" t="s">
-        <v>1174</v>
-      </c>
       <c r="F226" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G226" s="48"/>
       <c r="H226" s="52"/>
@@ -14567,19 +14573,19 @@
         <v>226</v>
       </c>
       <c r="B227" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C227" s="49" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D227" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E227" s="58" t="s">
         <v>1175</v>
       </c>
-      <c r="D227" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E227" s="58" t="s">
-        <v>1176</v>
-      </c>
       <c r="F227" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G227" s="48"/>
       <c r="H227" s="52"/>
@@ -14608,19 +14614,19 @@
         <v>227</v>
       </c>
       <c r="B228" s="48" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C228" s="49" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D228" s="54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E228" s="58" t="s">
         <v>1177</v>
       </c>
-      <c r="D228" s="54" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E228" s="58" t="s">
-        <v>1178</v>
-      </c>
       <c r="F228" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G228" s="48"/>
       <c r="H228" s="52"/>
@@ -14649,19 +14655,19 @@
         <v>228</v>
       </c>
       <c r="B229" s="48" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C229" s="49" t="s">
         <v>1179</v>
       </c>
-      <c r="C229" s="49" t="s">
+      <c r="D229" s="54" t="s">
         <v>1180</v>
       </c>
-      <c r="D229" s="54" t="s">
+      <c r="E229" s="58" t="s">
         <v>1181</v>
       </c>
-      <c r="E229" s="58" t="s">
-        <v>1182</v>
-      </c>
       <c r="F229" s="57" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G229" s="48"/>
       <c r="H229" s="52"/>
@@ -14690,19 +14696,19 @@
         <v>229</v>
       </c>
       <c r="B230" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C230" s="49" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D230" s="54" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E230" s="58" t="s">
         <v>1183</v>
       </c>
-      <c r="D230" s="54" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E230" s="58" t="s">
-        <v>1184</v>
-      </c>
       <c r="F230" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="231" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14710,19 +14716,19 @@
         <v>230</v>
       </c>
       <c r="B231" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C231" s="49" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D231" s="54" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E231" s="58" t="s">
         <v>1185</v>
       </c>
-      <c r="D231" s="54" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E231" s="58" t="s">
-        <v>1186</v>
-      </c>
       <c r="F231" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G231" s="48"/>
       <c r="H231" s="52"/>
@@ -14751,19 +14757,19 @@
         <v>231</v>
       </c>
       <c r="B232" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C232" s="49" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D232" s="54" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E232" s="58" t="s">
         <v>1187</v>
       </c>
-      <c r="D232" s="54" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E232" s="58" t="s">
-        <v>1188</v>
-      </c>
       <c r="F232" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G232" s="48"/>
       <c r="H232" s="52"/>
@@ -14792,19 +14798,19 @@
         <v>232</v>
       </c>
       <c r="B233" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C233" s="70" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="D233" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E233" s="58" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F233" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G233" s="48"/>
       <c r="H233" s="52"/>
@@ -14833,19 +14839,19 @@
         <v>233</v>
       </c>
       <c r="B234" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C234" s="49" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D234" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E234" s="58" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F234" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G234" s="48"/>
       <c r="H234" s="52"/>
@@ -14874,19 +14880,19 @@
         <v>234</v>
       </c>
       <c r="B235" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C235" s="49" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D235" s="54" t="s">
         <v>1190</v>
       </c>
-      <c r="D235" s="54" t="s">
+      <c r="E235" s="58" t="s">
         <v>1191</v>
       </c>
-      <c r="E235" s="58" t="s">
-        <v>1192</v>
-      </c>
       <c r="F235" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G235" s="48"/>
       <c r="H235" s="52"/>
@@ -14915,19 +14921,19 @@
         <v>235</v>
       </c>
       <c r="B236" s="48" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C236" s="49" t="s">
-        <v>1193</v>
+        <v>1178</v>
+      </c>
+      <c r="C236" s="70" t="s">
+        <v>1638</v>
       </c>
       <c r="D236" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E236" s="58" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="F236" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G236" s="48"/>
       <c r="H236" s="52"/>
@@ -14956,19 +14962,19 @@
         <v>236</v>
       </c>
       <c r="B237" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C237" s="49" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="D237" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E237" s="58" t="s">
         <v>966</v>
       </c>
       <c r="F237" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G237" s="48"/>
       <c r="H237" s="52"/>
@@ -14997,19 +15003,19 @@
         <v>237</v>
       </c>
       <c r="B238" s="48" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C238" s="49" t="s">
         <v>1179</v>
       </c>
-      <c r="C238" s="49" t="s">
+      <c r="D238" s="54" t="s">
         <v>1180</v>
-      </c>
-      <c r="D238" s="54" t="s">
-        <v>1181</v>
       </c>
       <c r="E238" s="58" t="s">
         <v>966</v>
       </c>
       <c r="F238" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G238" s="39"/>
       <c r="H238" s="42"/>
@@ -15038,19 +15044,19 @@
         <v>238</v>
       </c>
       <c r="B239" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C239" s="49" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="D239" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E239" s="40" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F239" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G239" s="39"/>
       <c r="H239" s="42"/>
@@ -15079,19 +15085,19 @@
         <v>239</v>
       </c>
       <c r="B240" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C240" s="49" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="D240" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E240" s="40" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="F240" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G240" s="39"/>
       <c r="H240" s="42"/>
@@ -15120,19 +15126,19 @@
         <v>240</v>
       </c>
       <c r="B241" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C241" s="49" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D241" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E241" s="40" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="F241" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G241" s="39"/>
       <c r="H241" s="42"/>
@@ -15161,19 +15167,19 @@
         <v>241</v>
       </c>
       <c r="B242" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C242" s="49" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D242" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E242" s="40" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="F242" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G242" s="39"/>
       <c r="H242" s="42"/>
@@ -15202,19 +15208,19 @@
         <v>242</v>
       </c>
       <c r="B243" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C243" s="49" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D243" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E243" s="40" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="F243" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G243" s="39"/>
       <c r="H243" s="42"/>
@@ -15243,19 +15249,19 @@
         <v>243</v>
       </c>
       <c r="B244" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C244" s="49" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="D244" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E244" s="40" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="F244" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G244" s="39"/>
       <c r="H244" s="42"/>
@@ -15284,19 +15290,19 @@
         <v>244</v>
       </c>
       <c r="B245" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C245" s="49" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="D245" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E245" s="40" t="s">
         <v>1066</v>
       </c>
       <c r="F245" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G245" s="39"/>
       <c r="H245" s="42"/>
@@ -15325,19 +15331,19 @@
         <v>245</v>
       </c>
       <c r="B246" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C246" s="49" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="D246" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E246" s="40" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="F246" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G246" s="39"/>
       <c r="H246" s="42"/>
@@ -15366,19 +15372,19 @@
         <v>246</v>
       </c>
       <c r="B247" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C247" s="49" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="D247" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E247" s="40" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F247" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G247" s="39"/>
       <c r="H247" s="42"/>
@@ -15407,19 +15413,19 @@
         <v>247</v>
       </c>
       <c r="B248" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C248" s="49" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D248" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E248" s="58" t="s">
         <v>1012</v>
       </c>
       <c r="F248" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G248" s="48"/>
       <c r="H248" s="52"/>
@@ -15448,19 +15454,19 @@
         <v>248</v>
       </c>
       <c r="B249" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C249" s="49" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="D249" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E249" s="40" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="F249" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G249" s="39"/>
       <c r="H249" s="42"/>
@@ -15489,19 +15495,19 @@
         <v>249</v>
       </c>
       <c r="B250" s="48" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C250" s="49" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="D250" s="54" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E250" s="40" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="F250" s="57" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G250" s="39"/>
       <c r="H250" s="42"/>
@@ -49341,17 +49347,17 @@
         <v>4</v>
       </c>
       <c r="C1" s="30" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1220</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="30" t="s">
         <v>1222</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>1224</v>
       </c>
       <c r="F1" s="31"/>
       <c r="G1" s="29" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -49374,7 +49380,7 @@
         <v>576</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="5"/>
@@ -49397,10 +49403,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>723</v>
@@ -49425,13 +49431,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E4" s="30" t="s">
         <v>1230</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>1231</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>1232</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="34"/>
@@ -49453,10 +49459,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>1236</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>1238</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="30"/>
@@ -49483,7 +49489,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="30" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="28"/>
@@ -49505,13 +49511,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="28"/>
@@ -49533,10 +49539,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="30" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>1236</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>1238</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="37"/>
@@ -49559,13 +49565,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="28"/>
@@ -49587,13 +49593,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="28"/>
@@ -49618,7 +49624,7 @@
         <v>1001</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>39</v>
@@ -49643,10 +49649,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="5"/>
@@ -49669,13 +49675,13 @@
         <v>16</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="28"/>
@@ -49697,10 +49703,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="29"/>
@@ -49727,7 +49733,7 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="30" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
@@ -49749,13 +49755,13 @@
         <v>20</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>1308</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>1310</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="30"/>
@@ -49802,13 +49808,13 @@
         <v>22</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="G18" s="35"/>
       <c r="H18" s="8"/>
@@ -49829,13 +49835,13 @@
         <v>23</v>
       </c>
       <c r="C19" s="30" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>1319</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>1320</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>1321</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="8"/>
@@ -49860,7 +49866,7 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="30" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="8"/>
@@ -49881,13 +49887,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="8"/>
@@ -49908,10 +49914,10 @@
         <v>26</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="E22" s="31"/>
       <c r="G22" s="5"/>
@@ -49933,13 +49939,13 @@
         <v>27</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>572</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="G23" s="36"/>
       <c r="H23" s="8"/>
@@ -49963,7 +49969,7 @@
         <v>841</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="E24" s="31"/>
       <c r="G24" s="5"/>
@@ -49985,13 +49991,13 @@
         <v>31</v>
       </c>
       <c r="C25" s="30" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>1345</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>1346</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>1347</v>
       </c>
       <c r="G25" s="30"/>
       <c r="H25" s="8"/>
@@ -50060,10 +50066,10 @@
         <v>34</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>768</v>
@@ -50087,10 +50093,10 @@
         <v>35</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="E29" s="31"/>
       <c r="G29" s="28"/>
@@ -50112,13 +50118,13 @@
         <v>36</v>
       </c>
       <c r="C30" s="30" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>1360</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="30" t="s">
         <v>1362</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>1364</v>
       </c>
       <c r="G30" s="28"/>
       <c r="H30" s="8"/>
@@ -50162,13 +50168,13 @@
         <v>39</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="G32" s="28"/>
       <c r="H32" s="8"/>
@@ -50189,10 +50195,10 @@
         <v>40</v>
       </c>
       <c r="C33" s="30" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>1360</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>1362</v>
       </c>
       <c r="E33" s="30" t="s">
         <v>790</v>
@@ -50216,13 +50222,13 @@
         <v>41</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="8"/>
@@ -50243,13 +50249,13 @@
         <v>42</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="8"/>
@@ -50274,7 +50280,7 @@
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="30" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="8"/>
@@ -50295,10 +50301,10 @@
         <v>44</v>
       </c>
       <c r="C37" s="30" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>1384</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>1386</v>
       </c>
       <c r="E37" s="31"/>
       <c r="G37" s="28"/>
@@ -50320,10 +50326,10 @@
         <v>45</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="E38" s="31"/>
       <c r="G38" s="28"/>
@@ -50345,13 +50351,13 @@
         <v>46</v>
       </c>
       <c r="C39" s="30" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>1391</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="30" t="s">
         <v>1393</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>1395</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="8"/>
@@ -50372,13 +50378,13 @@
         <v>49</v>
       </c>
       <c r="C40" s="30" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>1398</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>1400</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="8"/>
@@ -50399,13 +50405,13 @@
         <v>50</v>
       </c>
       <c r="C41" s="30" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>1401</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>1402</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>1403</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="8"/>
@@ -50426,13 +50432,13 @@
         <v>52</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="8"/>
@@ -50457,7 +50463,7 @@
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="30" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="8"/>
@@ -50478,13 +50484,13 @@
         <v>55</v>
       </c>
       <c r="C44" s="30" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>1414</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="30" t="s">
         <v>1416</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>1418</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="8"/>
@@ -50505,10 +50511,10 @@
         <v>56</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="E45" s="30" t="s">
         <v>841</v>
@@ -50532,13 +50538,13 @@
         <v>57</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>1424</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>1426</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>1428</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="8"/>
@@ -50559,13 +50565,13 @@
         <v>58</v>
       </c>
       <c r="C47" s="30" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>1430</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>1432</v>
-      </c>
       <c r="E47" s="30" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="8"/>
@@ -50586,13 +50592,13 @@
         <v>59</v>
       </c>
       <c r="C48" s="30" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>1434</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>1435</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>1436</v>
       </c>
       <c r="G48" s="28"/>
       <c r="H48" s="8"/>
@@ -50613,13 +50619,13 @@
         <v>60</v>
       </c>
       <c r="C49" s="30" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>1439</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="30" t="s">
         <v>1441</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>1443</v>
       </c>
       <c r="G49" s="28"/>
       <c r="H49" s="8"/>
@@ -50640,13 +50646,13 @@
         <v>61</v>
       </c>
       <c r="C50" s="30" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E50" s="30" t="s">
         <v>1446</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>1447</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>1448</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="8"/>
@@ -50667,10 +50673,10 @@
         <v>62</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="E51" s="31"/>
       <c r="G51" s="28"/>
@@ -50692,10 +50698,10 @@
         <v>63</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="E52" s="31"/>
       <c r="G52" s="28"/>
@@ -50723,7 +50729,7 @@
         <v>1022</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="G53" s="28"/>
       <c r="H53" s="8"/>
@@ -50747,10 +50753,10 @@
         <v>873</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="8"/>
@@ -50771,13 +50777,13 @@
         <v>68</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="G55" s="28"/>
       <c r="H55" s="8"/>
@@ -50798,13 +50804,13 @@
         <v>69</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="G56" s="28"/>
       <c r="H56" s="8"/>
@@ -50852,7 +50858,7 @@
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="30" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="G58" s="28"/>
       <c r="H58" s="8"/>
@@ -50900,7 +50906,7 @@
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="30" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="G60" s="28"/>
       <c r="H60" s="8"/>
@@ -51019,7 +51025,7 @@
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="30" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="G65" s="28"/>
       <c r="H65" s="8"/>
@@ -51044,7 +51050,7 @@
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="30" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="G66" s="28"/>
       <c r="H66" s="8"/>
@@ -51065,10 +51071,10 @@
         <v>83</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="E67" s="31"/>
       <c r="G67" s="28"/>
@@ -51090,13 +51096,13 @@
         <v>84</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="G68" s="28"/>
       <c r="H68" s="8"/>
@@ -51120,10 +51126,10 @@
         <v>924</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="G69" s="28"/>
       <c r="H69" s="8"/>
@@ -51170,7 +51176,7 @@
         <v>945</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="E71" s="31"/>
       <c r="G71" s="28"/>
@@ -51192,13 +51198,13 @@
         <v>90</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="G72" s="28"/>
       <c r="H72" s="8"/>
@@ -51219,13 +51225,13 @@
         <v>91</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="G73" s="28"/>
       <c r="H73" s="8"/>
@@ -51297,7 +51303,7 @@
         <v>945</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="E76" s="31"/>
       <c r="G76" s="28"/>
@@ -51323,7 +51329,7 @@
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="30" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="G77" s="28"/>
       <c r="H77" s="8"/>
@@ -51371,7 +51377,7 @@
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="30" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="G79" s="28"/>
       <c r="H79" s="8"/>
@@ -51392,10 +51398,10 @@
         <v>101</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="E80" s="31"/>
       <c r="G80" s="28"/>
@@ -51440,13 +51446,13 @@
         <v>103</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>1054</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="G82" s="28"/>
       <c r="H82" s="8"/>
@@ -51467,10 +51473,10 @@
         <v>106</v>
       </c>
       <c r="C83" s="30" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>1546</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>1548</v>
       </c>
       <c r="E83" s="31"/>
       <c r="G83" s="28"/>
@@ -51492,13 +51498,13 @@
         <v>107</v>
       </c>
       <c r="C84" s="30" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="G84" s="28"/>
       <c r="H84" s="8"/>
@@ -51519,13 +51525,13 @@
         <v>108</v>
       </c>
       <c r="C85" s="30" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="G85" s="28"/>
       <c r="H85" s="8"/>
@@ -51573,7 +51579,7 @@
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="30" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="8"/>
@@ -51621,7 +51627,7 @@
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="30" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="G89" s="28"/>
       <c r="H89" s="8"/>
@@ -51642,13 +51648,13 @@
         <v>113</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="G90" s="28"/>
       <c r="H90" s="8"/>
@@ -51669,7 +51675,7 @@
         <v>114</v>
       </c>
       <c r="C91" s="30" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>1054</v>
@@ -51721,7 +51727,7 @@
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="30" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G93" s="28"/>
       <c r="H93" s="8"/>
@@ -51746,7 +51752,7 @@
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="30" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="G94" s="28"/>
       <c r="H94" s="8"/>
@@ -51767,10 +51773,10 @@
         <v>118</v>
       </c>
       <c r="C95" s="30" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="E95" s="31"/>
       <c r="G95" s="28"/>
@@ -51792,13 +51798,13 @@
         <v>120</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="G96" s="28"/>
       <c r="H96" s="8"/>
@@ -51846,7 +51852,7 @@
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="30" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="G98" s="28"/>
       <c r="H98" s="8"/>
@@ -51867,13 +51873,13 @@
         <v>124</v>
       </c>
       <c r="C99" s="30" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G99" s="28"/>
       <c r="H99" s="8"/>
@@ -51898,7 +51904,7 @@
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="30" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="G100" s="28"/>
       <c r="H100" s="8"/>
@@ -51923,7 +51929,7 @@
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="30" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="G101" s="28"/>
       <c r="H101" s="8"/>
@@ -51996,7 +52002,7 @@
       </c>
       <c r="D104" s="8"/>
       <c r="E104" s="30" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="G104" s="28"/>
       <c r="H104" s="8"/>
@@ -52021,7 +52027,7 @@
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="30" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="G105" s="28"/>
       <c r="H105" s="8"/>
@@ -52046,7 +52052,7 @@
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="30" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="G106" s="28"/>
       <c r="H106" s="8"/>
@@ -52071,7 +52077,7 @@
       </c>
       <c r="D107" s="8"/>
       <c r="E107" s="30" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="G107" s="28"/>
       <c r="H107" s="8"/>
@@ -52144,7 +52150,7 @@
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="30" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G110" s="28"/>
       <c r="H110" s="8"/>
@@ -52169,7 +52175,7 @@
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="30" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="G111" s="28"/>
       <c r="H111" s="8"/>
@@ -52290,7 +52296,7 @@
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="30" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="G116" s="28"/>
       <c r="H116" s="8"/>
@@ -52315,7 +52321,7 @@
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="30" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="G117" s="28"/>
       <c r="H117" s="8"/>
@@ -52340,7 +52346,7 @@
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="30" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G118" s="28"/>
       <c r="H118" s="8"/>
@@ -52365,7 +52371,7 @@
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="30" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="G119" s="28"/>
       <c r="H119" s="8"/>
@@ -52392,7 +52398,7 @@
         <v>1056</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="G120" s="28"/>
       <c r="H120" s="8"/>
@@ -52417,7 +52423,7 @@
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="30" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="G121" s="28"/>
       <c r="H121" s="8"/>
@@ -52442,7 +52448,7 @@
       </c>
       <c r="D122" s="8"/>
       <c r="E122" s="30" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G122" s="28"/>
       <c r="H122" s="8"/>
@@ -52558,7 +52564,7 @@
         <v>1084</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="E127" s="30" t="s">
         <v>1084</v>
@@ -52628,13 +52634,13 @@
         <v>161</v>
       </c>
       <c r="C130" s="30" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="D130" s="5" t="s">
+        <v>1577</v>
+      </c>
+      <c r="E130" s="30" t="s">
         <v>1579</v>
-      </c>
-      <c r="E130" s="30" t="s">
-        <v>1581</v>
       </c>
       <c r="G130" s="28"/>
       <c r="H130" s="8"/>
@@ -52658,7 +52664,7 @@
         <v>1084</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="E131" s="31"/>
       <c r="G131" s="28"/>
@@ -52703,10 +52709,10 @@
         <v>164</v>
       </c>
       <c r="C133" s="30" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="E133" s="31"/>
       <c r="G133" s="28"/>
@@ -52849,7 +52855,7 @@
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="30" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="G139" s="28"/>
       <c r="H139" s="8"/>
@@ -67004,19 +67010,19 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="D1" s="30" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>1219</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1223</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1225</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -67287,10 +67293,10 @@
         <v>77</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -67304,10 +67310,10 @@
         <v>100</v>
       </c>
       <c r="D22" s="30" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>1235</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>1237</v>
       </c>
       <c r="H22" s="32"/>
     </row>
@@ -67322,10 +67328,10 @@
         <v>100</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="H23" s="32"/>
     </row>
@@ -67340,10 +67346,10 @@
         <v>100</v>
       </c>
       <c r="D24" s="30" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>1241</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>1243</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -67357,10 +67363,10 @@
         <v>100</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -67391,10 +67397,10 @@
         <v>100</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -67408,10 +67414,10 @@
         <v>100</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -67425,10 +67431,10 @@
         <v>94</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -67442,10 +67448,10 @@
         <v>94</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="H30" s="32"/>
     </row>
@@ -67460,10 +67466,10 @@
         <v>94</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="H31" s="32"/>
     </row>
@@ -67478,10 +67484,10 @@
         <v>94</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="H32" s="32"/>
     </row>
@@ -67496,10 +67502,10 @@
         <v>94</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="H33" s="32"/>
     </row>
@@ -67514,10 +67520,10 @@
         <v>111</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="H34" s="32"/>
     </row>
@@ -67532,10 +67538,10 @@
         <v>111</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="H35" s="32"/>
     </row>
@@ -67550,10 +67556,10 @@
         <v>117</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="H36" s="32"/>
     </row>
@@ -67568,10 +67574,10 @@
         <v>117</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="H37" s="32"/>
     </row>
@@ -67586,10 +67592,10 @@
         <v>117</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="H38" s="32"/>
     </row>
@@ -67604,10 +67610,10 @@
         <v>117</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="H39" s="32"/>
     </row>
@@ -67640,10 +67646,10 @@
         <v>128</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="H41" s="32"/>
     </row>
@@ -67658,10 +67664,10 @@
         <v>128</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -67711,10 +67717,10 @@
         <v>151</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="H45" s="32"/>
     </row>
@@ -67729,10 +67735,10 @@
         <v>151</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -67746,10 +67752,10 @@
         <v>151</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -67763,10 +67769,10 @@
         <v>151</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -67780,10 +67786,10 @@
         <v>151</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -67814,10 +67820,10 @@
         <v>157</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="H51" s="32"/>
     </row>
@@ -67850,10 +67856,10 @@
         <v>157</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="H53" s="32"/>
     </row>
@@ -67868,10 +67874,10 @@
         <v>157</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="H54" s="32"/>
     </row>
@@ -67886,10 +67892,10 @@
         <v>157</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="H55" s="32"/>
     </row>
@@ -67904,10 +67910,10 @@
         <v>157</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="H56" s="32"/>
     </row>
@@ -67922,10 +67928,10 @@
         <v>157</v>
       </c>
       <c r="D57" s="30" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E57" s="30" t="s">
         <v>1302</v>
-      </c>
-      <c r="E57" s="30" t="s">
-        <v>1304</v>
       </c>
       <c r="H57" s="32"/>
     </row>
@@ -67940,10 +67946,10 @@
         <v>157</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="H58" s="32"/>
     </row>
@@ -67958,10 +67964,10 @@
         <v>157</v>
       </c>
       <c r="D59" s="30" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E59" s="30" t="s">
         <v>1309</v>
-      </c>
-      <c r="E59" s="30" t="s">
-        <v>1311</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -67992,10 +67998,10 @@
         <v>157</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68009,10 +68015,10 @@
         <v>157</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -68023,13 +68029,13 @@
         <v>58</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E63" s="30" t="s">
         <v>1316</v>
-      </c>
-      <c r="D63" s="30" t="s">
-        <v>1317</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>1318</v>
       </c>
       <c r="H63" s="32"/>
     </row>
@@ -68044,10 +68050,10 @@
         <v>168</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="H64" s="32"/>
     </row>
@@ -68062,10 +68068,10 @@
         <v>168</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="H65" s="32"/>
     </row>
@@ -68080,10 +68086,10 @@
         <v>168</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="H66" s="32"/>
     </row>
@@ -68098,10 +68104,10 @@
         <v>168</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="H67" s="32"/>
     </row>
@@ -68116,10 +68122,10 @@
         <v>168</v>
       </c>
       <c r="D68" s="30" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E68" s="30" t="s">
         <v>1334</v>
-      </c>
-      <c r="E68" s="30" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -68133,10 +68139,10 @@
         <v>173</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="H69" s="32"/>
     </row>
@@ -68151,10 +68157,10 @@
         <v>173</v>
       </c>
       <c r="D70" s="30" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E70" s="30" t="s">
         <v>1340</v>
-      </c>
-      <c r="E70" s="30" t="s">
-        <v>1342</v>
       </c>
       <c r="H70" s="32"/>
     </row>
@@ -68169,10 +68175,10 @@
         <v>173</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="H71" s="32"/>
     </row>
@@ -68187,10 +68193,10 @@
         <v>173</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H72" s="32"/>
     </row>
@@ -68205,10 +68211,10 @@
         <v>173</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="H73" s="32"/>
     </row>
@@ -68223,10 +68229,10 @@
         <v>173</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="H74" s="32"/>
     </row>
@@ -68259,10 +68265,10 @@
         <v>173</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="H76" s="32"/>
     </row>
@@ -68277,10 +68283,10 @@
         <v>179</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="H77" s="32"/>
     </row>
@@ -68312,10 +68318,10 @@
         <v>179</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68329,10 +68335,10 @@
         <v>179</v>
       </c>
       <c r="D80" s="30" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E80" s="30" t="s">
         <v>1361</v>
-      </c>
-      <c r="E80" s="30" t="s">
-        <v>1363</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68381,10 +68387,10 @@
         <v>190</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="H83" s="32"/>
     </row>
@@ -68399,10 +68405,10 @@
         <v>190</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -68416,10 +68422,10 @@
         <v>195</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="H85" s="32"/>
     </row>
@@ -68434,10 +68440,10 @@
         <v>195</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="H86" s="32"/>
     </row>
@@ -68452,10 +68458,10 @@
         <v>195</v>
       </c>
       <c r="D87" s="30" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="H87" s="32"/>
     </row>
@@ -68470,10 +68476,10 @@
         <v>195</v>
       </c>
       <c r="D88" s="30" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="E88" s="30" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="H88" s="32"/>
     </row>
@@ -68488,10 +68494,10 @@
         <v>195</v>
       </c>
       <c r="D89" s="30" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="H89" s="32"/>
     </row>
@@ -68506,10 +68512,10 @@
         <v>195</v>
       </c>
       <c r="D90" s="30" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E90" s="30" t="s">
         <v>1383</v>
-      </c>
-      <c r="E90" s="30" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68540,10 +68546,10 @@
         <v>195</v>
       </c>
       <c r="D92" s="30" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68557,10 +68563,10 @@
         <v>195</v>
       </c>
       <c r="D93" s="30" t="s">
+        <v>1390</v>
+      </c>
+      <c r="E93" s="30" t="s">
         <v>1392</v>
-      </c>
-      <c r="E93" s="30" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -68574,10 +68580,10 @@
         <v>201</v>
       </c>
       <c r="D94" s="30" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="H94" s="32"/>
     </row>
@@ -68610,10 +68616,10 @@
         <v>201</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68627,10 +68633,10 @@
         <v>201</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68644,10 +68650,10 @@
         <v>201</v>
       </c>
       <c r="D98" s="30" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68661,10 +68667,10 @@
         <v>201</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68678,10 +68684,10 @@
         <v>201</v>
       </c>
       <c r="D100" s="30" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E100" s="30" t="s">
         <v>1415</v>
-      </c>
-      <c r="E100" s="30" t="s">
-        <v>1417</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68695,10 +68701,10 @@
         <v>201</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68712,10 +68718,10 @@
         <v>201</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -68729,10 +68735,10 @@
         <v>201</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -68746,10 +68752,10 @@
         <v>209</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="H104" s="32"/>
     </row>
@@ -68764,10 +68770,10 @@
         <v>209</v>
       </c>
       <c r="D105" s="30" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E105" s="30" t="s">
         <v>1429</v>
-      </c>
-      <c r="E105" s="30" t="s">
-        <v>1431</v>
       </c>
       <c r="H105" s="32"/>
     </row>
@@ -68800,10 +68806,10 @@
         <v>209</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="H107" s="32"/>
     </row>
@@ -68818,10 +68824,10 @@
         <v>209</v>
       </c>
       <c r="D108" s="30" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E108" s="30" t="s">
         <v>1440</v>
-      </c>
-      <c r="E108" s="30" t="s">
-        <v>1442</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -68835,10 +68841,10 @@
         <v>213</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="H109" s="32"/>
     </row>
@@ -68871,10 +68877,10 @@
         <v>213</v>
       </c>
       <c r="D111" s="30" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="H111" s="32"/>
     </row>
@@ -68889,10 +68895,10 @@
         <v>213</v>
       </c>
       <c r="D112" s="30" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E112" s="30" t="s">
         <v>1451</v>
-      </c>
-      <c r="E112" s="30" t="s">
-        <v>1453</v>
       </c>
       <c r="H112" s="32"/>
     </row>
@@ -68961,10 +68967,10 @@
         <v>213</v>
       </c>
       <c r="D116" s="30" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="H116" s="32"/>
     </row>
@@ -68997,10 +69003,10 @@
         <v>213</v>
       </c>
       <c r="D118" s="30" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="H118" s="32"/>
     </row>
@@ -69015,10 +69021,10 @@
         <v>213</v>
       </c>
       <c r="D119" s="30" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69032,10 +69038,10 @@
         <v>213</v>
       </c>
       <c r="D120" s="30" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69049,10 +69055,10 @@
         <v>213</v>
       </c>
       <c r="D121" s="30" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69066,10 +69072,10 @@
         <v>213</v>
       </c>
       <c r="D122" s="30" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69083,10 +69089,10 @@
         <v>213</v>
       </c>
       <c r="D123" s="30" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69100,10 +69106,10 @@
         <v>213</v>
       </c>
       <c r="D124" s="30" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69117,10 +69123,10 @@
         <v>213</v>
       </c>
       <c r="D125" s="30" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69134,10 +69140,10 @@
         <v>213</v>
       </c>
       <c r="D126" s="30" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69151,10 +69157,10 @@
         <v>213</v>
       </c>
       <c r="D127" s="30" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69185,10 +69191,10 @@
         <v>213</v>
       </c>
       <c r="D129" s="30" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="E129" s="30" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69202,10 +69208,10 @@
         <v>213</v>
       </c>
       <c r="D130" s="30" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="E130" s="30" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69219,10 +69225,10 @@
         <v>213</v>
       </c>
       <c r="D131" s="30" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="E131" s="30" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69236,10 +69242,10 @@
         <v>213</v>
       </c>
       <c r="D132" s="30" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="E132" s="30" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69288,10 +69294,10 @@
         <v>217</v>
       </c>
       <c r="D135" s="30" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="E135" s="30" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="H135" s="32"/>
     </row>
@@ -69306,10 +69312,10 @@
         <v>217</v>
       </c>
       <c r="D136" s="30" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="E136" s="30" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="H136" s="32"/>
     </row>
@@ -69324,10 +69330,10 @@
         <v>225</v>
       </c>
       <c r="D137" s="30" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="E137" s="30" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="H137" s="32"/>
     </row>
@@ -69342,10 +69348,10 @@
         <v>225</v>
       </c>
       <c r="D138" s="30" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="E138" s="30" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="H138" s="32"/>
     </row>
@@ -69360,10 +69366,10 @@
         <v>225</v>
       </c>
       <c r="D139" s="30" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="E139" s="30" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -69377,10 +69383,10 @@
         <v>229</v>
       </c>
       <c r="D140" s="30" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="E140" s="30" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="H140" s="32"/>
     </row>
@@ -69395,10 +69401,10 @@
         <v>229</v>
       </c>
       <c r="D141" s="30" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="E141" s="30" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="H141" s="32"/>
     </row>
@@ -69413,10 +69419,10 @@
         <v>233</v>
       </c>
       <c r="D142" s="30" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="E142" s="30" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="H142" s="32"/>
     </row>
@@ -69431,10 +69437,10 @@
         <v>233</v>
       </c>
       <c r="D143" s="30" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="E143" s="30" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="H143" s="32"/>
     </row>
@@ -69449,10 +69455,10 @@
         <v>233</v>
       </c>
       <c r="D144" s="30" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="E144" s="30" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="H144" s="32"/>
     </row>
@@ -69467,10 +69473,10 @@
         <v>233</v>
       </c>
       <c r="D145" s="30" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="E145" s="30" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69484,10 +69490,10 @@
         <v>239</v>
       </c>
       <c r="D146" s="30" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="E146" s="30" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69501,10 +69507,10 @@
         <v>239</v>
       </c>
       <c r="D147" s="30" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="E147" s="30" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -69536,10 +69542,10 @@
         <v>244</v>
       </c>
       <c r="D149" s="30" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="E149" s="30" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="H149" s="32"/>
     </row>
@@ -69554,10 +69560,10 @@
         <v>246</v>
       </c>
       <c r="D150" s="30" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="E150" s="30" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="H150" s="32"/>
     </row>
@@ -69572,10 +69578,10 @@
         <v>246</v>
       </c>
       <c r="D151" s="30" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="E151" s="30" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="H151" s="32"/>
     </row>
@@ -69590,10 +69596,10 @@
         <v>258</v>
       </c>
       <c r="D152" s="30" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="E152" s="30" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="H152" s="32"/>
     </row>
@@ -69608,10 +69614,10 @@
         <v>258</v>
       </c>
       <c r="D153" s="30" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="E153" s="30" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69642,10 +69648,10 @@
         <v>258</v>
       </c>
       <c r="D155" s="30" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="E155" s="30" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69659,10 +69665,10 @@
         <v>258</v>
       </c>
       <c r="D156" s="30" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="E156" s="30" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69693,10 +69699,10 @@
         <v>264</v>
       </c>
       <c r="D158" s="30" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="E158" s="30" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69710,10 +69716,10 @@
         <v>264</v>
       </c>
       <c r="D159" s="30" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="E159" s="30" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69727,10 +69733,10 @@
         <v>264</v>
       </c>
       <c r="D160" s="30" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E160" s="30" t="s">
         <v>1545</v>
-      </c>
-      <c r="E160" s="30" t="s">
-        <v>1547</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69744,10 +69750,10 @@
         <v>264</v>
       </c>
       <c r="D161" s="30" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="E161" s="30" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69761,10 +69767,10 @@
         <v>264</v>
       </c>
       <c r="D162" s="30" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="E162" s="30" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69778,10 +69784,10 @@
         <v>270</v>
       </c>
       <c r="D163" s="30" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="E163" s="30" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69795,10 +69801,10 @@
         <v>270</v>
       </c>
       <c r="D164" s="30" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="E164" s="30" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -69812,10 +69818,10 @@
         <v>270</v>
       </c>
       <c r="D165" s="30" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="E165" s="30" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="166" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>